<commit_message>
Start filling list of current variables
</commit_message>
<xml_diff>
--- a/design/variable_naming_convention.xlsx
+++ b/design/variable_naming_convention.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukeolfman/Programs/craps-game/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED728CE8-5F29-6845-9B0F-2AB7B3E7267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62002FA-B7CF-C347-88D5-C94EAF5D4334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{723B574F-FE27-604D-8FF0-17BE9AB32048}"/>
+    <workbookView xWindow="41980" yWindow="2100" windowWidth="28040" windowHeight="17440" xr2:uid="{723B574F-FE27-604D-8FF0-17BE9AB32048}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>For</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>const/let</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>let</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>camel</t>
+  </si>
+  <si>
+    <t>Current Name</t>
+  </si>
+  <si>
+    <t>New Name</t>
+  </si>
+  <si>
+    <t>playerMoney</t>
+  </si>
+  <si>
+    <t>lastPlayerMoney</t>
+  </si>
+  <si>
+    <t>playerRoll</t>
+  </si>
+  <si>
+    <t>playerPoint</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Track player's money</t>
+  </si>
+  <si>
+    <t>Track last dice roll</t>
+  </si>
+  <si>
+    <t>Track current point</t>
   </si>
 </sst>
 </file>
@@ -91,6 +142,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11C49CD8-B6EA-7F46-8FD9-8896D98DA70E}" name="Table1" displayName="Table1" ref="A1:G14" totalsRowShown="0">
+  <autoFilter ref="A1:G14" xr:uid="{11C49CD8-B6EA-7F46-8FD9-8896D98DA70E}"/>
+  <tableColumns count="7">
+    <tableColumn id="6" xr3:uid="{6E938C40-B4FD-8947-A21A-3A41F98EBDC4}" name="Current Name"/>
+    <tableColumn id="1" xr3:uid="{8EAB4389-D0A4-F14B-8160-47786EA2460E}" name="const/let"/>
+    <tableColumn id="2" xr3:uid="{578FCB33-8AED-7F4B-A58A-1D398E45975E}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{C52FCE2F-366D-7642-A028-8F933F45A197}" name="Location"/>
+    <tableColumn id="4" xr3:uid="{6C55B05C-7748-5A4B-AC99-FE415061E985}" name="Case"/>
+    <tableColumn id="5" xr3:uid="{4E1DD17D-DF02-CB4B-8195-7E623FC21BFF}" name="New Name"/>
+    <tableColumn id="8" xr3:uid="{8331ED6B-4FFA-D445-8868-57A72C5CD2EB}" name="Usage"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,18 +477,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9239AB-C9B9-1E4D-AF47-C40F2ED083A9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>